<commit_message>
GP model updated 2
</commit_message>
<xml_diff>
--- a/model_Grain/Grain_lookup.xlsx
+++ b/model_Grain/Grain_lookup.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4664D65-2A4B-48A8-AC10-8CB13AE112AE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{407F13F7-5B34-484B-8BFF-891FD06B6918}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="12" state="hidden" r:id="rId1"/>
@@ -411,10 +411,10 @@
     <numFmt numFmtId="164" formatCode="0.0E+00"/>
     <numFmt numFmtId="165" formatCode="0.000"/>
     <numFmt numFmtId="166" formatCode="0.0"/>
-    <numFmt numFmtId="168" formatCode="0.0000"/>
-    <numFmt numFmtId="169" formatCode="&quot;$&quot;#,##0"/>
-    <numFmt numFmtId="170" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="171" formatCode="&quot;$&quot;#,##0.0"/>
+    <numFmt numFmtId="167" formatCode="0.0000"/>
+    <numFmt numFmtId="168" formatCode="&quot;$&quot;#,##0"/>
+    <numFmt numFmtId="169" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="170" formatCode="&quot;$&quot;#,##0.0"/>
   </numFmts>
   <fonts count="8" x14ac:knownFonts="1">
     <font>
@@ -554,7 +554,7 @@
     <xf numFmtId="44" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="113">
+  <cellXfs count="109">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -602,10 +602,10 @@
     <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="169" fontId="0" fillId="5" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="0" fillId="5" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="171" fontId="0" fillId="5" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="170" fontId="0" fillId="5" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -639,7 +639,7 @@
     <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="168" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -672,7 +672,7 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="2" fontId="1" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -745,7 +745,7 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="168" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="11" fontId="0" fillId="6" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
@@ -763,27 +763,12 @@
     <xf numFmtId="11" fontId="0" fillId="5" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="11" fontId="1" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="11" fontId="1" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="11" fontId="0" fillId="6" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="11" fontId="0" fillId="6" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -794,7 +779,7 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="168" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -805,12 +790,6 @@
     </xf>
     <xf numFmtId="2" fontId="1" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="1" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -847,7 +826,7 @@
     <xf numFmtId="11" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -873,6 +852,15 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -1172,14 +1160,14 @@
   <sheetData>
     <row r="2" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B2" s="9"/>
-      <c r="C2" s="76" t="s">
+      <c r="C2" s="106" t="s">
         <v>32</v>
       </c>
-      <c r="D2" s="76"/>
-      <c r="E2" s="76"/>
-      <c r="F2" s="76"/>
-      <c r="G2" s="76"/>
-      <c r="H2" s="76"/>
+      <c r="D2" s="106"/>
+      <c r="E2" s="106"/>
+      <c r="F2" s="106"/>
+      <c r="G2" s="106"/>
+      <c r="H2" s="106"/>
     </row>
     <row r="3" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B3" s="9"/>
@@ -1559,14 +1547,14 @@
     </row>
     <row r="19" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B19" s="9"/>
-      <c r="C19" s="76" t="s">
+      <c r="C19" s="106" t="s">
         <v>45</v>
       </c>
-      <c r="D19" s="76"/>
-      <c r="E19" s="76"/>
-      <c r="F19" s="76"/>
-      <c r="G19" s="76"/>
-      <c r="H19" s="76"/>
+      <c r="D19" s="106"/>
+      <c r="E19" s="106"/>
+      <c r="F19" s="106"/>
+      <c r="G19" s="106"/>
+      <c r="H19" s="106"/>
       <c r="I19" s="9"/>
       <c r="J19" s="9"/>
     </row>
@@ -1813,8 +1801,8 @@
   </sheetPr>
   <dimension ref="A1:N51"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="I40" sqref="I40"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1822,9 +1810,9 @@
     <col min="1" max="1" width="21.7109375" style="22" customWidth="1"/>
     <col min="2" max="2" width="29.5703125" style="8" customWidth="1"/>
     <col min="3" max="3" width="62.85546875" style="22" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.85546875" style="95" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.140625" style="95" bestFit="1" customWidth="1"/>
-    <col min="6" max="8" width="13.85546875" style="95" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.85546875" style="88" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.140625" style="88" bestFit="1" customWidth="1"/>
+    <col min="6" max="8" width="13.85546875" style="88" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="9.140625" style="22"/>
     <col min="10" max="10" width="24" style="22" customWidth="1"/>
     <col min="11" max="11" width="12" style="22" bestFit="1" customWidth="1"/>
@@ -1855,7 +1843,7 @@
       </c>
     </row>
     <row r="2" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="77" t="s">
+      <c r="A2" s="107" t="s">
         <v>69</v>
       </c>
       <c r="B2" s="11" t="s">
@@ -1864,24 +1852,24 @@
       <c r="C2" s="25" t="s">
         <v>52</v>
       </c>
-      <c r="D2" s="79">
+      <c r="D2" s="74">
         <f>D3*24*330</f>
         <v>673200</v>
       </c>
-      <c r="E2" s="79">
+      <c r="E2" s="74">
         <f t="shared" ref="E2" si="0">E3*24*330</f>
         <v>950400</v>
       </c>
-      <c r="F2" s="79">
+      <c r="F2" s="74">
         <v>1702800</v>
       </c>
-      <c r="G2" s="79">
+      <c r="G2" s="74">
         <v>2098800</v>
       </c>
-      <c r="H2" s="79">
+      <c r="H2" s="74">
         <v>4997520</v>
       </c>
-      <c r="I2" s="96">
+      <c r="I2" s="89">
         <v>0</v>
       </c>
       <c r="J2" s="22" t="s">
@@ -1889,29 +1877,29 @@
       </c>
     </row>
     <row r="3" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="77"/>
+      <c r="A3" s="107"/>
       <c r="B3" s="11" t="s">
         <v>0</v>
       </c>
       <c r="C3" s="25" t="s">
         <v>53</v>
       </c>
-      <c r="D3" s="80">
+      <c r="D3" s="75">
         <v>85</v>
       </c>
-      <c r="E3" s="79">
+      <c r="E3" s="74">
         <v>120</v>
       </c>
-      <c r="F3" s="79">
+      <c r="F3" s="74">
         <v>215</v>
       </c>
-      <c r="G3" s="79">
+      <c r="G3" s="74">
         <v>265</v>
       </c>
-      <c r="H3" s="79">
+      <c r="H3" s="74">
         <v>631</v>
       </c>
-      <c r="I3" s="96">
+      <c r="I3" s="89">
         <v>1</v>
       </c>
       <c r="J3" s="22" t="s">
@@ -1919,29 +1907,29 @@
       </c>
     </row>
     <row r="4" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="77"/>
+      <c r="A4" s="107"/>
       <c r="B4" s="11" t="s">
         <v>0</v>
       </c>
       <c r="C4" s="25" t="s">
         <v>9</v>
       </c>
-      <c r="D4" s="80">
+      <c r="D4" s="75">
         <v>0.26</v>
       </c>
-      <c r="E4" s="79">
+      <c r="E4" s="74">
         <v>0.26</v>
       </c>
-      <c r="F4" s="79">
+      <c r="F4" s="74">
         <v>0.26</v>
       </c>
-      <c r="G4" s="79">
+      <c r="G4" s="74">
         <v>0.26</v>
       </c>
-      <c r="H4" s="79">
+      <c r="H4" s="74">
         <v>0.26</v>
       </c>
-      <c r="I4" s="96">
+      <c r="I4" s="89">
         <v>2</v>
       </c>
       <c r="J4" s="22" t="s">
@@ -1949,34 +1937,34 @@
       </c>
     </row>
     <row r="5" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="77"/>
+      <c r="A5" s="107"/>
       <c r="B5" s="12" t="s">
         <v>50</v>
       </c>
       <c r="C5" s="27" t="s">
         <v>59</v>
       </c>
-      <c r="D5" s="81">
+      <c r="D5" s="76">
         <f>371143.15/D2</f>
         <v>0.55131186868686877</v>
       </c>
-      <c r="E5" s="81">
+      <c r="E5" s="76">
         <f>526247.75/E2</f>
         <v>0.55371185816498314</v>
       </c>
-      <c r="F5" s="81">
+      <c r="F5" s="76">
         <f>941706.5/F2</f>
         <v>0.55303412027249232</v>
       </c>
-      <c r="G5" s="81">
+      <c r="G5" s="76">
         <f>1163284.5/G2</f>
         <v>0.55426172098341908</v>
       </c>
-      <c r="H5" s="81">
+      <c r="H5" s="76">
         <f>2769725/H2</f>
         <v>0.55421989306696118</v>
       </c>
-      <c r="I5" s="96">
+      <c r="I5" s="89">
         <v>3</v>
       </c>
       <c r="J5" s="22" t="s">
@@ -1984,34 +1972,34 @@
       </c>
     </row>
     <row r="6" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="77"/>
+      <c r="A6" s="107"/>
       <c r="B6" s="12" t="s">
         <v>50</v>
       </c>
       <c r="C6" s="27" t="s">
         <v>60</v>
       </c>
-      <c r="D6" s="81">
+      <c r="D6" s="76">
         <f>133364/D2</f>
         <v>0.19810457516339869</v>
       </c>
-      <c r="E6" s="81">
+      <c r="E6" s="76">
         <f>189099/E2</f>
         <v>0.19896780303030304</v>
       </c>
-      <c r="F6" s="81">
+      <c r="F6" s="76">
         <f>338388/F2</f>
         <v>0.19872445384073292</v>
       </c>
-      <c r="G6" s="81">
+      <c r="G6" s="76">
         <f>417999/G2</f>
         <v>0.1991609491137793</v>
       </c>
-      <c r="H6" s="81">
+      <c r="H6" s="76">
         <f>995233/H2</f>
         <v>0.19914537610654884</v>
       </c>
-      <c r="I6" s="96">
+      <c r="I6" s="89">
         <v>4</v>
       </c>
       <c r="J6" s="22" t="s">
@@ -2019,34 +2007,34 @@
       </c>
     </row>
     <row r="7" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="77"/>
+      <c r="A7" s="107"/>
       <c r="B7" s="12" t="s">
         <v>50</v>
       </c>
       <c r="C7" s="27" t="s">
         <v>61</v>
       </c>
-      <c r="D7" s="81">
+      <c r="D7" s="76">
         <f>42431/D2</f>
         <v>6.3028817587641117E-2</v>
       </c>
-      <c r="E7" s="81">
+      <c r="E7" s="76">
         <f>60163/E2</f>
         <v>6.3302819865319868E-2</v>
       </c>
-      <c r="F7" s="81">
+      <c r="F7" s="76">
         <f>107660/F2</f>
         <v>6.3225276015973692E-2</v>
       </c>
-      <c r="G7" s="81">
+      <c r="G7" s="76">
         <f>132992/G2</f>
         <v>6.3365732799695068E-2</v>
       </c>
-      <c r="H7" s="81">
+      <c r="H7" s="76">
         <f>316647/H2</f>
         <v>6.3360826970177211E-2</v>
       </c>
-      <c r="I7" s="96">
+      <c r="I7" s="89">
         <v>5</v>
       </c>
       <c r="J7" s="22" t="s">
@@ -2054,116 +2042,116 @@
       </c>
     </row>
     <row r="8" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="77"/>
+      <c r="A8" s="107"/>
       <c r="B8" s="12" t="s">
         <v>50</v>
       </c>
       <c r="C8" s="27" t="s">
         <v>62</v>
       </c>
-      <c r="D8" s="81">
+      <c r="D8" s="76">
         <f>44675910/D2/1000</f>
         <v>6.6363502673796787E-2</v>
       </c>
-      <c r="E8" s="81">
+      <c r="E8" s="76">
         <f>63346439/E2/1000</f>
         <v>6.6652397937710439E-2</v>
       </c>
-      <c r="F8" s="81">
+      <c r="F8" s="76">
         <f>113356786/F2/1000</f>
         <v>6.6570816302560482E-2</v>
       </c>
-      <c r="G8" s="81">
+      <c r="G8" s="76">
         <f>140028971/1000/G2</f>
         <v>6.6718587287974071E-2</v>
       </c>
-      <c r="H8" s="81">
+      <c r="H8" s="76">
         <f>333402311/1000/H2</f>
         <v>6.671355212185244E-2</v>
       </c>
-      <c r="I8" s="96">
+      <c r="I8" s="89">
         <v>6</v>
       </c>
     </row>
     <row r="9" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="77"/>
+      <c r="A9" s="107"/>
       <c r="B9" s="13" t="s">
         <v>3</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="D9" s="107">
+      <c r="D9" s="100">
         <v>140.76808805970148</v>
       </c>
-      <c r="E9" s="107">
+      <c r="E9" s="100">
         <v>134.11094736842105</v>
       </c>
-      <c r="F9" s="107">
+      <c r="F9" s="100">
         <v>129.03465882352941</v>
       </c>
-      <c r="G9" s="107">
+      <c r="G9" s="100">
         <v>127.90855000000001</v>
       </c>
-      <c r="H9" s="107">
+      <c r="H9" s="100">
         <v>124.2127266</v>
       </c>
-      <c r="I9" s="96">
+      <c r="I9" s="89">
         <v>7</v>
       </c>
-      <c r="J9" s="82"/>
-    </row>
-    <row r="10" spans="1:14" s="82" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="77"/>
+      <c r="J9" s="77"/>
+    </row>
+    <row r="10" spans="1:14" s="77" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="107"/>
       <c r="B10" s="13" t="s">
         <v>3</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="D10" s="107">
+      <c r="D10" s="100">
         <v>2633.1053684179105</v>
       </c>
-      <c r="E10" s="107">
+      <c r="E10" s="100">
         <v>2633.098804336842</v>
       </c>
-      <c r="F10" s="107">
+      <c r="F10" s="100">
         <v>2633.1448937999999</v>
       </c>
-      <c r="G10" s="107">
+      <c r="G10" s="100">
         <v>2633.0941504380953</v>
       </c>
-      <c r="H10" s="107">
+      <c r="H10" s="100">
         <v>2633.0984711599999</v>
       </c>
-      <c r="I10" s="96">
+      <c r="I10" s="89">
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:14" s="82" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="77"/>
+    <row r="11" spans="1:14" s="77" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="107"/>
       <c r="B11" s="14" t="s">
         <v>4</v>
       </c>
       <c r="C11" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="D11" s="83">
+      <c r="D11" s="78">
         <v>1.5940000000000001</v>
       </c>
-      <c r="E11" s="83">
+      <c r="E11" s="78">
         <v>1.1279999999999999</v>
       </c>
-      <c r="F11" s="84">
+      <c r="F11" s="79">
         <v>0.86899999999999999</v>
       </c>
-      <c r="G11" s="84">
+      <c r="G11" s="79">
         <v>0.79500000000000004</v>
       </c>
-      <c r="H11" s="84">
+      <c r="H11" s="79">
         <v>0.60799999999999998</v>
       </c>
-      <c r="I11" s="96">
+      <c r="I11" s="89">
         <v>9</v>
       </c>
       <c r="J11" s="22"/>
@@ -2172,30 +2160,30 @@
       <c r="M11" s="22"/>
       <c r="N11" s="22"/>
     </row>
-    <row r="12" spans="1:14" s="82" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="77"/>
-      <c r="B12" s="85" t="s">
+    <row r="12" spans="1:14" s="77" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="107"/>
+      <c r="B12" s="80" t="s">
         <v>27</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D12" s="86">
-        <v>11.83</v>
-      </c>
-      <c r="E12" s="87">
-        <v>11.94</v>
-      </c>
-      <c r="F12" s="87">
-        <v>11.9</v>
-      </c>
-      <c r="G12" s="88">
-        <v>11.92</v>
-      </c>
-      <c r="H12" s="88">
-        <v>11.89</v>
-      </c>
-      <c r="I12" s="96">
+      <c r="D12" s="81">
+        <v>12</v>
+      </c>
+      <c r="E12" s="81">
+        <v>12</v>
+      </c>
+      <c r="F12" s="81">
+        <v>12</v>
+      </c>
+      <c r="G12" s="81">
+        <v>12</v>
+      </c>
+      <c r="H12" s="81">
+        <v>12</v>
+      </c>
+      <c r="I12" s="89">
         <v>10</v>
       </c>
       <c r="J12" s="22"/>
@@ -2204,8 +2192,8 @@
       <c r="M12" s="22"/>
       <c r="N12" s="22"/>
     </row>
-    <row r="13" spans="1:14" s="82" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="77"/>
+    <row r="13" spans="1:14" s="77" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="107"/>
       <c r="B13" s="15" t="s">
         <v>15</v>
       </c>
@@ -2227,7 +2215,7 @@
       <c r="H13" s="67">
         <v>434431200</v>
       </c>
-      <c r="I13" s="96">
+      <c r="I13" s="89">
         <v>11</v>
       </c>
       <c r="J13" s="22"/>
@@ -2236,8 +2224,8 @@
       <c r="M13" s="22"/>
       <c r="N13" s="22"/>
     </row>
-    <row r="14" spans="1:14" s="82" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="77"/>
+    <row r="14" spans="1:14" s="77" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="107"/>
       <c r="B14" s="15" t="s">
         <v>15</v>
       </c>
@@ -2250,7 +2238,7 @@
       <c r="E14" s="67">
         <v>108767000</v>
       </c>
-      <c r="F14" s="75">
+      <c r="F14" s="73">
         <v>185824000</v>
       </c>
       <c r="G14" s="67">
@@ -2259,7 +2247,7 @@
       <c r="H14" s="67">
         <v>413744000</v>
       </c>
-      <c r="I14" s="96">
+      <c r="I14" s="89">
         <v>12</v>
       </c>
       <c r="J14" s="22"/>
@@ -2268,8 +2256,8 @@
       <c r="M14" s="22"/>
       <c r="N14" s="22"/>
     </row>
-    <row r="15" spans="1:14" s="82" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="77"/>
+    <row r="15" spans="1:14" s="77" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="107"/>
       <c r="B15" s="15" t="s">
         <v>15</v>
       </c>
@@ -2291,7 +2279,7 @@
       <c r="H15" s="67">
         <v>866662804</v>
       </c>
-      <c r="I15" s="96">
+      <c r="I15" s="89">
         <v>13</v>
       </c>
       <c r="J15" s="22"/>
@@ -2300,8 +2288,8 @@
       <c r="M15" s="22"/>
       <c r="N15" s="22"/>
     </row>
-    <row r="16" spans="1:14" s="82" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="77"/>
+    <row r="16" spans="1:14" s="77" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="107"/>
       <c r="B16" s="15" t="s">
         <v>15</v>
       </c>
@@ -2314,7 +2302,7 @@
       <c r="E16" s="67">
         <v>19775485</v>
       </c>
-      <c r="F16" s="75">
+      <c r="F16" s="73">
         <v>34521417</v>
       </c>
       <c r="G16" s="67">
@@ -2323,7 +2311,7 @@
       <c r="H16" s="67">
         <v>99110343</v>
       </c>
-      <c r="I16" s="96">
+      <c r="I16" s="89">
         <v>14</v>
       </c>
       <c r="J16" s="22"/>
@@ -2333,7 +2321,7 @@
       <c r="N16" s="22"/>
     </row>
     <row r="17" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="77"/>
+      <c r="A17" s="107"/>
       <c r="B17" s="15" t="s">
         <v>15</v>
       </c>
@@ -2346,7 +2334,7 @@
       <c r="E17" s="67">
         <v>131284454.91891894</v>
       </c>
-      <c r="F17" s="75">
+      <c r="F17" s="73">
         <v>235217981.72972974</v>
       </c>
       <c r="G17" s="67">
@@ -2355,12 +2343,12 @@
       <c r="H17" s="67">
         <v>690337425.44864869</v>
       </c>
-      <c r="I17" s="96">
+      <c r="I17" s="89">
         <v>15</v>
       </c>
     </row>
     <row r="18" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="77"/>
+      <c r="A18" s="107"/>
       <c r="B18" s="15" t="s">
         <v>15</v>
       </c>
@@ -2373,7 +2361,7 @@
       <c r="E18" s="67">
         <v>20559000</v>
       </c>
-      <c r="F18" s="75">
+      <c r="F18" s="73">
         <v>28800000</v>
       </c>
       <c r="G18" s="67">
@@ -2382,12 +2370,12 @@
       <c r="H18" s="67">
         <v>64335000</v>
       </c>
-      <c r="I18" s="96">
+      <c r="I18" s="89">
         <v>16</v>
       </c>
     </row>
     <row r="19" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="77"/>
+      <c r="A19" s="107"/>
       <c r="B19" s="21" t="s">
         <v>15</v>
       </c>
@@ -2409,18 +2397,18 @@
       <c r="H19" s="67">
         <v>9738035.5513513088</v>
       </c>
-      <c r="I19" s="96">
+      <c r="I19" s="89">
         <v>17</v>
       </c>
     </row>
     <row r="20" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="77" t="s">
+      <c r="A20" s="107" t="s">
         <v>29</v>
       </c>
       <c r="B20" s="12" t="s">
         <v>49</v>
       </c>
-      <c r="C20" s="89" t="s">
+      <c r="C20" s="82" t="s">
         <v>63</v>
       </c>
       <c r="D20" s="69">
@@ -2443,16 +2431,16 @@
         <f>7780.321*1000</f>
         <v>7780321</v>
       </c>
-      <c r="I20" s="96">
+      <c r="I20" s="89">
         <v>18</v>
       </c>
     </row>
     <row r="21" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="77"/>
+      <c r="A21" s="107"/>
       <c r="B21" s="12" t="s">
         <v>49</v>
       </c>
-      <c r="C21" s="89" t="s">
+      <c r="C21" s="82" t="s">
         <v>51</v>
       </c>
       <c r="D21" s="69">
@@ -2475,23 +2463,23 @@
         <f>32773.182*(1-0.099518)*1000</f>
         <v>29511660.473724</v>
       </c>
-      <c r="I21" s="96">
+      <c r="I21" s="89">
         <v>19</v>
       </c>
     </row>
     <row r="22" spans="1:14" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="77"/>
+      <c r="A22" s="107"/>
       <c r="B22" s="12" t="s">
         <v>49</v>
       </c>
-      <c r="C22" s="90" t="s">
+      <c r="C22" s="83" t="s">
         <v>67</v>
       </c>
-      <c r="D22" s="91">
+      <c r="D22" s="84">
         <f>D20/(D2*1000)</f>
         <v>1.548663101604278E-3</v>
       </c>
-      <c r="E22" s="91">
+      <c r="E22" s="84">
         <f>E20/(E2*1000)</f>
         <v>1.5554082491582492E-3</v>
       </c>
@@ -2507,12 +2495,12 @@
         <f>H20/(H2*1000)</f>
         <v>1.5568363908498616E-3</v>
       </c>
-      <c r="I22" s="96">
+      <c r="I22" s="89">
         <v>20</v>
       </c>
     </row>
     <row r="23" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="77"/>
+      <c r="A23" s="107"/>
       <c r="B23" s="16" t="s">
         <v>27</v>
       </c>
@@ -2524,12 +2512,12 @@
       <c r="F23" s="71"/>
       <c r="G23" s="71"/>
       <c r="H23" s="71"/>
-      <c r="I23" s="96">
+      <c r="I23" s="89">
         <v>21</v>
       </c>
     </row>
     <row r="24" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="77"/>
+      <c r="A24" s="107"/>
       <c r="B24" s="16" t="s">
         <v>27</v>
       </c>
@@ -2541,16 +2529,16 @@
       <c r="F24" s="71"/>
       <c r="G24" s="71"/>
       <c r="H24" s="71"/>
-      <c r="I24" s="96">
+      <c r="I24" s="89">
         <v>22</v>
       </c>
     </row>
     <row r="25" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="77"/>
+      <c r="A25" s="107"/>
       <c r="B25" s="16" t="s">
         <v>27</v>
       </c>
-      <c r="C25" s="92" t="s">
+      <c r="C25" s="85" t="s">
         <v>54</v>
       </c>
       <c r="D25" s="70"/>
@@ -2558,24 +2546,34 @@
       <c r="F25" s="70"/>
       <c r="G25" s="70"/>
       <c r="H25" s="70"/>
-      <c r="I25" s="96">
+      <c r="I25" s="89">
         <v>23</v>
       </c>
     </row>
-    <row r="26" spans="1:14" s="94" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="77"/>
+    <row r="26" spans="1:14" s="87" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="107"/>
       <c r="B26" s="16" t="s">
         <v>27</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="D26" s="72"/>
-      <c r="E26" s="73"/>
-      <c r="F26" s="73"/>
-      <c r="G26" s="73"/>
-      <c r="H26" s="73"/>
-      <c r="I26" s="96">
+        <v>14</v>
+      </c>
+      <c r="D26" s="42">
+        <v>2.5</v>
+      </c>
+      <c r="E26" s="42">
+        <v>2.5</v>
+      </c>
+      <c r="F26" s="42">
+        <v>2.5</v>
+      </c>
+      <c r="G26" s="42">
+        <v>2.5</v>
+      </c>
+      <c r="H26" s="42">
+        <v>2.5</v>
+      </c>
+      <c r="I26" s="89">
         <v>24</v>
       </c>
       <c r="J26" s="22"/>
@@ -2585,174 +2583,174 @@
       <c r="N26" s="22"/>
     </row>
     <row r="27" spans="1:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="77"/>
+      <c r="A27" s="107"/>
       <c r="B27" s="20" t="s">
         <v>50</v>
       </c>
       <c r="C27" s="27" t="s">
         <v>59</v>
       </c>
-      <c r="D27" s="111">
+      <c r="D27" s="104">
         <f>371143.15/D2</f>
         <v>0.55131186868686877</v>
       </c>
-      <c r="E27" s="111">
+      <c r="E27" s="104">
         <f>526247.75/E2</f>
         <v>0.55371185816498314</v>
       </c>
-      <c r="F27" s="111">
+      <c r="F27" s="104">
         <f>F5</f>
         <v>0.55303412027249232</v>
       </c>
-      <c r="G27" s="111">
+      <c r="G27" s="104">
         <f>G5</f>
         <v>0.55426172098341908</v>
       </c>
-      <c r="H27" s="111">
+      <c r="H27" s="104">
         <f>H5</f>
         <v>0.55421989306696118</v>
       </c>
-      <c r="I27" s="96">
+      <c r="I27" s="89">
         <v>25</v>
       </c>
     </row>
     <row r="28" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="77"/>
+      <c r="A28" s="107"/>
       <c r="B28" s="20" t="s">
         <v>50</v>
       </c>
       <c r="C28" s="27" t="s">
         <v>60</v>
       </c>
-      <c r="D28" s="111">
+      <c r="D28" s="104">
         <f>130153/D2</f>
         <v>0.19333481877599526</v>
       </c>
-      <c r="E28" s="111">
+      <c r="E28" s="104">
         <f>184545/E2</f>
         <v>0.19417613636363637</v>
       </c>
-      <c r="F28" s="111">
+      <c r="F28" s="104">
         <f>330238/F2</f>
         <v>0.19393821940333569</v>
       </c>
-      <c r="G28" s="111">
+      <c r="G28" s="104">
         <f>407936/G2</f>
         <v>0.1943663045549838</v>
       </c>
-      <c r="H28" s="111">
+      <c r="H28" s="104">
         <f>971273/H2</f>
         <v>0.19435099809505516</v>
       </c>
-      <c r="I28" s="96">
+      <c r="I28" s="89">
         <v>26</v>
       </c>
     </row>
     <row r="29" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="77"/>
+      <c r="A29" s="107"/>
       <c r="B29" s="20" t="s">
         <v>50</v>
       </c>
       <c r="C29" s="27" t="s">
         <v>61</v>
       </c>
-      <c r="D29" s="111">
+      <c r="D29" s="104">
         <f>42431/D2</f>
         <v>6.3028817587641117E-2</v>
       </c>
-      <c r="E29" s="111">
+      <c r="E29" s="104">
         <f>60163/E2</f>
         <v>6.3302819865319868E-2</v>
       </c>
-      <c r="F29" s="111">
-        <f>F7</f>
+      <c r="F29" s="104">
+        <f t="shared" ref="F29:H30" si="1">F7</f>
         <v>6.3225276015973692E-2</v>
       </c>
-      <c r="G29" s="111">
-        <f>G7</f>
+      <c r="G29" s="104">
+        <f t="shared" si="1"/>
         <v>6.3365732799695068E-2</v>
       </c>
-      <c r="H29" s="111">
-        <f>H7</f>
+      <c r="H29" s="104">
+        <f t="shared" si="1"/>
         <v>6.3360826970177211E-2</v>
       </c>
-      <c r="I29" s="96">
+      <c r="I29" s="89">
         <v>27</v>
       </c>
     </row>
     <row r="30" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="77"/>
+      <c r="A30" s="107"/>
       <c r="B30" s="20" t="s">
         <v>50</v>
       </c>
       <c r="C30" s="27" t="s">
         <v>62</v>
       </c>
-      <c r="D30" s="111">
+      <c r="D30" s="104">
         <f>44675910/D2/1000</f>
         <v>6.6363502673796787E-2</v>
       </c>
-      <c r="E30" s="111">
+      <c r="E30" s="104">
         <f>63346439/E2/1000</f>
         <v>6.6652397937710439E-2</v>
       </c>
-      <c r="F30" s="111">
-        <f>F8</f>
+      <c r="F30" s="104">
+        <f t="shared" si="1"/>
         <v>6.6570816302560482E-2</v>
       </c>
-      <c r="G30" s="111">
-        <f>G8</f>
+      <c r="G30" s="104">
+        <f t="shared" si="1"/>
         <v>6.6718587287974071E-2</v>
       </c>
-      <c r="H30" s="111">
-        <f>H8</f>
+      <c r="H30" s="104">
+        <f t="shared" si="1"/>
         <v>6.671355212185244E-2</v>
       </c>
-      <c r="I30" s="96">
+      <c r="I30" s="89">
         <v>28</v>
       </c>
     </row>
     <row r="31" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="77"/>
+      <c r="A31" s="107"/>
       <c r="B31" s="20" t="s">
         <v>18</v>
       </c>
       <c r="C31" s="39" t="s">
         <v>54</v>
       </c>
-      <c r="D31" s="97"/>
-      <c r="E31" s="97"/>
-      <c r="F31" s="97"/>
-      <c r="G31" s="97"/>
-      <c r="H31" s="97"/>
-      <c r="I31" s="96">
+      <c r="D31" s="90"/>
+      <c r="E31" s="90"/>
+      <c r="F31" s="90"/>
+      <c r="G31" s="90"/>
+      <c r="H31" s="90"/>
+      <c r="I31" s="89">
         <v>29</v>
       </c>
     </row>
-    <row r="32" spans="1:14" s="82" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="77"/>
+    <row r="32" spans="1:14" s="77" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="107"/>
       <c r="B32" s="13" t="s">
         <v>3</v>
       </c>
       <c r="C32" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D32" s="107">
+      <c r="D32" s="100">
         <v>1.3172865671641603</v>
       </c>
-      <c r="E32" s="107">
+      <c r="E32" s="100">
         <v>1.1546199999999942</v>
       </c>
-      <c r="F32" s="107">
+      <c r="F32" s="100">
         <v>0.99335058823530176</v>
       </c>
-      <c r="G32" s="107">
+      <c r="G32" s="100">
         <v>0.92722666666664111</v>
       </c>
-      <c r="H32" s="107">
+      <c r="H32" s="100">
         <v>0.8369904000000048</v>
       </c>
-      <c r="I32" s="96">
+      <c r="I32" s="89">
         <v>30</v>
       </c>
       <c r="J32" s="22"/>
@@ -2761,30 +2759,30 @@
       <c r="M32" s="22"/>
       <c r="N32" s="22"/>
     </row>
-    <row r="33" spans="1:14" s="82" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="77"/>
+    <row r="33" spans="1:14" s="77" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="107"/>
       <c r="B33" s="13" t="s">
         <v>3</v>
       </c>
       <c r="C33" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D33" s="107">
+      <c r="D33" s="100">
         <v>40.180464119403041</v>
       </c>
-      <c r="E33" s="107">
+      <c r="E33" s="100">
         <v>40.212223663157602</v>
       </c>
-      <c r="F33" s="107">
+      <c r="F33" s="100">
         <v>40.225714058823542</v>
       </c>
-      <c r="G33" s="107">
+      <c r="G33" s="100">
         <v>40.263099238095037</v>
       </c>
-      <c r="H33" s="107">
+      <c r="H33" s="100">
         <v>40.19335474799982</v>
       </c>
-      <c r="I33" s="96">
+      <c r="I33" s="89">
         <v>31</v>
       </c>
       <c r="J33" s="22"/>
@@ -2793,20 +2791,20 @@
       <c r="M33" s="22"/>
       <c r="N33" s="22"/>
     </row>
-    <row r="34" spans="1:14" s="82" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="77"/>
+    <row r="34" spans="1:14" s="77" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="107"/>
       <c r="B34" s="14" t="s">
         <v>4</v>
       </c>
       <c r="C34" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="D34" s="98"/>
-      <c r="E34" s="98"/>
-      <c r="F34" s="99"/>
-      <c r="G34" s="99"/>
-      <c r="H34" s="99"/>
-      <c r="I34" s="96">
+      <c r="D34" s="91"/>
+      <c r="E34" s="91"/>
+      <c r="F34" s="92"/>
+      <c r="G34" s="92"/>
+      <c r="H34" s="92"/>
+      <c r="I34" s="89">
         <v>32</v>
       </c>
       <c r="J34" s="22"/>
@@ -2816,7 +2814,7 @@
       <c r="N34" s="22"/>
     </row>
     <row r="35" spans="1:14" ht="15" x14ac:dyDescent="0.25">
-      <c r="A35" s="77"/>
+      <c r="A35" s="107"/>
       <c r="B35" s="19" t="s">
         <v>70</v>
       </c>
@@ -2826,7 +2824,7 @@
       <c r="D35" s="57">
         <v>7669200</v>
       </c>
-      <c r="E35" s="101">
+      <c r="E35" s="94">
         <v>9454200</v>
       </c>
       <c r="F35" s="67">
@@ -2835,17 +2833,17 @@
       <c r="G35" s="67">
         <v>15208200</v>
       </c>
-      <c r="H35" s="101">
+      <c r="H35" s="94">
         <v>25141200</v>
       </c>
-      <c r="I35" s="96">
+      <c r="I35" s="89">
         <v>33</v>
       </c>
-      <c r="J35" s="102"/>
-      <c r="K35" s="100"/>
+      <c r="J35" s="95"/>
+      <c r="K35" s="93"/>
     </row>
     <row r="36" spans="1:14" ht="15" x14ac:dyDescent="0.25">
-      <c r="A36" s="77"/>
+      <c r="A36" s="107"/>
       <c r="B36" s="19" t="s">
         <v>70</v>
       </c>
@@ -2855,7 +2853,7 @@
       <c r="D36" s="57">
         <v>7304000</v>
       </c>
-      <c r="E36" s="101">
+      <c r="E36" s="94">
         <v>9004000</v>
       </c>
       <c r="F36" s="67">
@@ -2864,16 +2862,16 @@
       <c r="G36" s="67">
         <v>14484000</v>
       </c>
-      <c r="H36" s="101">
+      <c r="H36" s="94">
         <v>23944000</v>
       </c>
-      <c r="I36" s="96">
+      <c r="I36" s="89">
         <v>34</v>
       </c>
-      <c r="K36" s="102"/>
+      <c r="K36" s="95"/>
     </row>
     <row r="37" spans="1:14" ht="15" x14ac:dyDescent="0.25">
-      <c r="A37" s="77"/>
+      <c r="A37" s="107"/>
       <c r="B37" s="19" t="s">
         <v>70</v>
       </c>
@@ -2881,27 +2879,27 @@
         <v>72</v>
       </c>
       <c r="D37" s="57">
-        <v>1909649</v>
-      </c>
-      <c r="E37" s="101">
-        <v>2477379</v>
-      </c>
-      <c r="F37" s="101">
-        <v>3849904</v>
+        <v>1225061</v>
+      </c>
+      <c r="E37" s="94">
+        <v>1633141</v>
+      </c>
+      <c r="F37" s="94">
+        <v>2665990</v>
       </c>
       <c r="G37" s="67">
-        <v>4549718</v>
+        <v>3206420</v>
       </c>
       <c r="H37" s="57">
-        <v>9108894</v>
-      </c>
-      <c r="I37" s="96">
+        <v>6898226</v>
+      </c>
+      <c r="I37" s="89">
         <v>35</v>
       </c>
-      <c r="K37" s="102"/>
+      <c r="K37" s="95"/>
     </row>
     <row r="38" spans="1:14" ht="15" x14ac:dyDescent="0.25">
-      <c r="A38" s="77"/>
+      <c r="A38" s="107"/>
       <c r="B38" s="19" t="s">
         <v>70</v>
       </c>
@@ -2911,10 +2909,10 @@
       <c r="D38" s="57">
         <v>158874</v>
       </c>
-      <c r="E38" s="101">
+      <c r="E38" s="94">
         <v>209914</v>
       </c>
-      <c r="F38" s="101">
+      <c r="F38" s="94">
         <v>348522</v>
       </c>
       <c r="G38" s="67">
@@ -2923,12 +2921,12 @@
       <c r="H38" s="67">
         <v>945832</v>
       </c>
-      <c r="I38" s="96">
+      <c r="I38" s="89">
         <v>36</v>
       </c>
     </row>
     <row r="39" spans="1:14" ht="15" x14ac:dyDescent="0.25">
-      <c r="A39" s="77"/>
+      <c r="A39" s="107"/>
       <c r="B39" s="19" t="s">
         <v>70</v>
       </c>
@@ -2938,10 +2936,10 @@
       <c r="D39" s="57">
         <v>0</v>
       </c>
-      <c r="E39" s="101">
+      <c r="E39" s="94">
         <v>0</v>
       </c>
-      <c r="F39" s="101">
+      <c r="F39" s="94">
         <v>0</v>
       </c>
       <c r="G39" s="67">
@@ -2950,39 +2948,39 @@
       <c r="H39" s="67">
         <v>0</v>
       </c>
-      <c r="I39" s="96">
+      <c r="I39" s="89">
         <v>37</v>
       </c>
     </row>
     <row r="40" spans="1:14" ht="15" x14ac:dyDescent="0.25">
-      <c r="A40" s="77"/>
+      <c r="A40" s="107"/>
       <c r="B40" s="19" t="s">
         <v>70</v>
       </c>
       <c r="C40" s="5" t="s">
         <v>75</v>
       </c>
-      <c r="D40" s="74">
-        <v>1163000</v>
-      </c>
-      <c r="E40" s="74">
-        <v>1434000</v>
-      </c>
-      <c r="F40" s="74">
-        <v>2010000</v>
+      <c r="D40" s="72">
+        <v>478412</v>
+      </c>
+      <c r="E40" s="72">
+        <v>589762</v>
+      </c>
+      <c r="F40" s="72">
+        <v>826086</v>
       </c>
       <c r="G40" s="67">
-        <v>2292000</v>
+        <v>948702</v>
       </c>
       <c r="H40" s="67">
-        <v>3779000</v>
-      </c>
-      <c r="I40" s="96">
+        <v>1568332</v>
+      </c>
+      <c r="I40" s="89">
         <v>38</v>
       </c>
     </row>
     <row r="41" spans="1:14" ht="15" x14ac:dyDescent="0.25">
-      <c r="A41" s="77"/>
+      <c r="A41" s="107"/>
       <c r="B41" s="19" t="s">
         <v>70</v>
       </c>
@@ -2992,10 +2990,10 @@
       <c r="D41" s="57">
         <v>587775</v>
       </c>
-      <c r="E41" s="101">
+      <c r="E41" s="94">
         <v>833465</v>
       </c>
-      <c r="F41" s="101">
+      <c r="F41" s="94">
         <v>1491382</v>
       </c>
       <c r="G41" s="67">
@@ -3004,93 +3002,93 @@
       <c r="H41" s="67">
         <v>4384062</v>
       </c>
-      <c r="I41" s="96">
+      <c r="I41" s="89">
         <v>39</v>
       </c>
     </row>
     <row r="42" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B42" s="7"/>
       <c r="C42" s="4"/>
-      <c r="D42" s="103"/>
-      <c r="E42" s="103"/>
-      <c r="F42" s="103"/>
-      <c r="G42" s="103"/>
+      <c r="D42" s="96"/>
+      <c r="E42" s="96"/>
+      <c r="F42" s="96"/>
+      <c r="G42" s="96"/>
       <c r="H42" s="41"/>
     </row>
     <row r="43" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B43" s="7"/>
-      <c r="C43" s="104"/>
-      <c r="D43" s="103"/>
-      <c r="E43" s="96"/>
-      <c r="F43" s="96"/>
-      <c r="G43" s="96"/>
-      <c r="H43" s="96"/>
+      <c r="C43" s="97"/>
+      <c r="D43" s="96"/>
+      <c r="E43" s="89"/>
+      <c r="F43" s="89"/>
+      <c r="G43" s="89"/>
+      <c r="H43" s="89"/>
     </row>
     <row r="44" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B44" s="7"/>
-      <c r="C44" s="104"/>
-      <c r="D44" s="103"/>
-      <c r="E44" s="96"/>
-      <c r="F44" s="96"/>
-      <c r="G44" s="96"/>
-      <c r="H44" s="96"/>
+      <c r="C44" s="97"/>
+      <c r="D44" s="96"/>
+      <c r="E44" s="89"/>
+      <c r="F44" s="89"/>
+      <c r="G44" s="89"/>
+      <c r="H44" s="89"/>
     </row>
     <row r="45" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B45" s="7"/>
-      <c r="E45" s="96"/>
-      <c r="F45" s="96"/>
-      <c r="G45" s="96"/>
-      <c r="H45" s="96"/>
+      <c r="E45" s="89"/>
+      <c r="F45" s="89"/>
+      <c r="G45" s="89"/>
+      <c r="H45" s="89"/>
     </row>
     <row r="46" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B46" s="7"/>
-      <c r="E46" s="96"/>
-      <c r="F46" s="96"/>
-      <c r="G46" s="96"/>
-      <c r="H46" s="96"/>
+      <c r="E46" s="89"/>
+      <c r="F46" s="89"/>
+      <c r="G46" s="89"/>
+      <c r="H46" s="89"/>
     </row>
     <row r="47" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B47" s="7"/>
-      <c r="E47" s="96"/>
-      <c r="F47" s="96"/>
-      <c r="G47" s="96"/>
-      <c r="H47" s="96"/>
+      <c r="E47" s="89"/>
+      <c r="F47" s="89"/>
+      <c r="G47" s="89"/>
+      <c r="H47" s="89"/>
     </row>
     <row r="48" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B48" s="7"/>
       <c r="C48" s="4"/>
-      <c r="D48" s="103"/>
-      <c r="E48" s="96"/>
-      <c r="F48" s="96"/>
-      <c r="G48" s="96"/>
-      <c r="H48" s="96"/>
+      <c r="D48" s="96"/>
+      <c r="E48" s="89"/>
+      <c r="F48" s="89"/>
+      <c r="G48" s="89"/>
+      <c r="H48" s="89"/>
     </row>
     <row r="49" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B49" s="7"/>
       <c r="C49" s="4"/>
-      <c r="D49" s="103"/>
-      <c r="E49" s="96"/>
-      <c r="F49" s="96"/>
-      <c r="G49" s="96"/>
-      <c r="H49" s="96"/>
+      <c r="D49" s="96"/>
+      <c r="E49" s="89"/>
+      <c r="F49" s="89"/>
+      <c r="G49" s="89"/>
+      <c r="H49" s="89"/>
     </row>
     <row r="50" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B50" s="7"/>
       <c r="C50" s="4"/>
-      <c r="D50" s="103"/>
-      <c r="E50" s="96"/>
-      <c r="F50" s="96"/>
-      <c r="G50" s="96"/>
-      <c r="H50" s="96"/>
+      <c r="D50" s="96"/>
+      <c r="E50" s="89"/>
+      <c r="F50" s="89"/>
+      <c r="G50" s="89"/>
+      <c r="H50" s="89"/>
     </row>
     <row r="51" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B51" s="6"/>
-      <c r="C51" s="82"/>
-      <c r="D51" s="96"/>
-      <c r="E51" s="96"/>
-      <c r="F51" s="96"/>
-      <c r="G51" s="96"/>
-      <c r="H51" s="96"/>
+      <c r="C51" s="77"/>
+      <c r="D51" s="89"/>
+      <c r="E51" s="89"/>
+      <c r="F51" s="89"/>
+      <c r="G51" s="89"/>
+      <c r="H51" s="89"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -3106,8 +3104,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D48B63FF-275C-4E59-A879-8F35A881D7FE}">
   <dimension ref="A1:K41"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="J17" sqref="J17"/>
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="I2" sqref="I2:I41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3115,11 +3113,11 @@
     <col min="1" max="1" width="18.85546875" style="22" customWidth="1"/>
     <col min="2" max="2" width="32.140625" style="23" customWidth="1"/>
     <col min="3" max="3" width="62.140625" style="22" customWidth="1"/>
-    <col min="4" max="4" width="15.7109375" style="95" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.42578125" style="95" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.85546875" style="105" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.42578125" style="105" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.7109375" style="105" customWidth="1"/>
+    <col min="4" max="4" width="15.7109375" style="88" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.42578125" style="88" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.85546875" style="98" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.42578125" style="98" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.7109375" style="98" customWidth="1"/>
     <col min="9" max="9" width="9.140625" style="22"/>
     <col min="10" max="10" width="35" style="22" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="21.28515625" style="22" bestFit="1" customWidth="1"/>
@@ -3151,7 +3149,7 @@
       </c>
     </row>
     <row r="2" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="78" t="s">
+      <c r="A2" s="108" t="s">
         <v>69</v>
       </c>
       <c r="B2" s="24" t="s">
@@ -3179,12 +3177,15 @@
         <f>2629770</f>
         <v>2629770</v>
       </c>
+      <c r="I2" s="22">
+        <v>0</v>
+      </c>
       <c r="J2" s="22" t="s">
         <v>92</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="78"/>
+      <c r="A3" s="108"/>
       <c r="B3" s="24" t="s">
         <v>0</v>
       </c>
@@ -3211,12 +3212,15 @@
         <f>H2/330/24</f>
         <v>332.04166666666669</v>
       </c>
+      <c r="I3" s="22">
+        <v>1</v>
+      </c>
       <c r="J3" s="22" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="4" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="78"/>
+      <c r="A4" s="108"/>
       <c r="B4" s="24" t="s">
         <v>0</v>
       </c>
@@ -3238,12 +3242,15 @@
       <c r="H4" s="26">
         <v>0.26</v>
       </c>
+      <c r="I4" s="22">
+        <v>2</v>
+      </c>
       <c r="J4" s="22" t="s">
         <v>94</v>
       </c>
     </row>
     <row r="5" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="78"/>
+      <c r="A5" s="108"/>
       <c r="B5" s="20" t="s">
         <v>18</v>
       </c>
@@ -3270,12 +3277,15 @@
         <f>896036351/$J$11/H$2</f>
         <v>114.00785788911755</v>
       </c>
+      <c r="I5" s="22">
+        <v>3</v>
+      </c>
       <c r="J5" s="22" t="s">
         <v>95</v>
       </c>
     </row>
     <row r="6" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="78"/>
+      <c r="A6" s="108"/>
       <c r="B6" s="20" t="s">
         <v>18</v>
       </c>
@@ -3302,12 +3312,15 @@
         <f>765534/H2*1000</f>
         <v>291.10302421884802</v>
       </c>
+      <c r="I6" s="22">
+        <v>4</v>
+      </c>
       <c r="J6" s="22" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="7" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="78"/>
+      <c r="A7" s="108"/>
       <c r="B7" s="20" t="s">
         <v>18</v>
       </c>
@@ -3334,12 +3347,15 @@
         <f>25535105/H2</f>
         <v>9.7100145640113009</v>
       </c>
+      <c r="I7" s="22">
+        <v>5</v>
+      </c>
       <c r="J7" s="22" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8" s="78"/>
+      <c r="A8" s="108"/>
       <c r="B8" s="20" t="s">
         <v>18</v>
       </c>
@@ -3351,7 +3367,10 @@
       <c r="F8" s="40"/>
       <c r="G8" s="40"/>
       <c r="H8" s="40"/>
-      <c r="J8" s="93">
+      <c r="I8" s="22">
+        <v>6</v>
+      </c>
+      <c r="J8" s="86">
         <v>358489485</v>
       </c>
       <c r="K8" s="22" t="s">
@@ -3359,29 +3378,32 @@
       </c>
     </row>
     <row r="9" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="78"/>
+      <c r="A9" s="108"/>
       <c r="B9" s="28" t="s">
         <v>3</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="D9" s="106">
+      <c r="D9" s="99">
         <v>92.870166131907311</v>
       </c>
-      <c r="E9" s="106">
+      <c r="E9" s="99">
         <v>76.432148306595366</v>
       </c>
-      <c r="F9" s="106">
+      <c r="F9" s="99">
         <v>71.98683177933178</v>
       </c>
-      <c r="G9" s="106">
+      <c r="G9" s="99">
         <v>63.832588472964943</v>
       </c>
-      <c r="H9" s="106">
+      <c r="H9" s="99">
         <v>62.33816379379185</v>
       </c>
-      <c r="J9" s="108">
+      <c r="I9" s="22">
+        <v>7</v>
+      </c>
+      <c r="J9" s="101">
         <v>117503006.20036501</v>
       </c>
       <c r="K9" s="22" t="s">
@@ -3389,29 +3411,32 @@
       </c>
     </row>
     <row r="10" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="78"/>
+      <c r="A10" s="108"/>
       <c r="B10" s="28" t="s">
         <v>3</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="D10" s="106">
+      <c r="D10" s="99">
         <v>647.63005632798581</v>
       </c>
-      <c r="E10" s="106">
+      <c r="E10" s="99">
         <v>647.45552946880571</v>
       </c>
-      <c r="F10" s="106">
+      <c r="F10" s="99">
         <v>661.3871509518259</v>
       </c>
-      <c r="G10" s="106">
+      <c r="G10" s="99">
         <v>647.34168579916809</v>
       </c>
-      <c r="H10" s="106">
+      <c r="H10" s="99">
         <v>647.3307055445913</v>
       </c>
-      <c r="J10" s="109">
+      <c r="I10" s="22">
+        <v>8</v>
+      </c>
+      <c r="J10" s="102">
         <f>J8/J9</f>
         <v>3.0508962842083132</v>
       </c>
@@ -3420,7 +3445,7 @@
       </c>
     </row>
     <row r="11" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="78"/>
+      <c r="A11" s="108"/>
       <c r="B11" s="29" t="s">
         <v>4</v>
       </c>
@@ -3432,7 +3457,10 @@
       <c r="F11" s="30"/>
       <c r="G11" s="60"/>
       <c r="H11" s="60"/>
-      <c r="J11" s="109">
+      <c r="I11" s="22">
+        <v>9</v>
+      </c>
+      <c r="J11" s="102">
         <f>0.789/0.264</f>
         <v>2.9886363636363638</v>
       </c>
@@ -3441,7 +3469,7 @@
       </c>
     </row>
     <row r="12" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="78"/>
+      <c r="A12" s="108"/>
       <c r="B12" s="31" t="s">
         <v>27</v>
       </c>
@@ -3449,24 +3477,27 @@
         <v>13</v>
       </c>
       <c r="D12" s="42">
-        <v>9.31</v>
+        <v>9</v>
       </c>
       <c r="E12" s="42">
-        <v>9.31</v>
+        <v>9</v>
       </c>
       <c r="F12" s="42">
-        <v>9.31</v>
+        <v>9</v>
       </c>
       <c r="G12" s="42">
-        <v>9.31</v>
+        <v>9</v>
       </c>
       <c r="H12" s="42">
-        <v>9.31</v>
-      </c>
-      <c r="K12" s="112"/>
+        <v>9</v>
+      </c>
+      <c r="I12" s="22">
+        <v>10</v>
+      </c>
+      <c r="K12" s="105"/>
     </row>
     <row r="13" spans="1:11" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="78"/>
+      <c r="A13" s="108"/>
       <c r="B13" s="19" t="s">
         <v>15</v>
       </c>
@@ -3488,12 +3519,15 @@
       <c r="H13" s="57">
         <v>434393400</v>
       </c>
-      <c r="J13" s="112" t="s">
+      <c r="I13" s="22">
+        <v>11</v>
+      </c>
+      <c r="J13" s="105" t="s">
         <v>111</v>
       </c>
     </row>
     <row r="14" spans="1:11" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="78"/>
+      <c r="A14" s="108"/>
       <c r="B14" s="19" t="s">
         <v>15</v>
       </c>
@@ -3520,15 +3554,18 @@
         <f>103427000*4</f>
         <v>413708000</v>
       </c>
-      <c r="J14" s="110">
+      <c r="I14" s="22">
+        <v>12</v>
+      </c>
+      <c r="J14" s="103">
         <v>358489485</v>
       </c>
-      <c r="K14" s="112" t="s">
+      <c r="K14" s="105" t="s">
         <v>112</v>
       </c>
     </row>
     <row r="15" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="78"/>
+      <c r="A15" s="108"/>
       <c r="B15" s="19" t="s">
         <v>15</v>
       </c>
@@ -3550,16 +3587,19 @@
       <c r="H15" s="57">
         <v>496748544</v>
       </c>
-      <c r="J15" s="112">
+      <c r="I15" s="22">
+        <v>13</v>
+      </c>
+      <c r="J15" s="105">
         <f>J14/0.789</f>
         <v>454359296.57794672</v>
       </c>
-      <c r="K15" s="112" t="s">
+      <c r="K15" s="105" t="s">
         <v>113</v>
       </c>
     </row>
     <row r="16" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="78"/>
+      <c r="A16" s="108"/>
       <c r="B16" s="19" t="s">
         <v>15</v>
       </c>
@@ -3581,16 +3621,19 @@
       <c r="H16" s="57">
         <v>67649867</v>
       </c>
-      <c r="J16" s="112">
+      <c r="I16" s="22">
+        <v>14</v>
+      </c>
+      <c r="J16" s="105">
         <f>J15*0.264</f>
         <v>119950854.29657795</v>
       </c>
-      <c r="K16" s="112" t="s">
+      <c r="K16" s="105" t="s">
         <v>114</v>
       </c>
     </row>
     <row r="17" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="78"/>
+      <c r="A17" s="108"/>
       <c r="B17" s="19" t="s">
         <v>15</v>
       </c>
@@ -3612,9 +3655,12 @@
       <c r="H17" s="57">
         <v>363265910.15585589</v>
       </c>
+      <c r="I17" s="22">
+        <v>15</v>
+      </c>
     </row>
     <row r="18" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="78"/>
+      <c r="A18" s="108"/>
       <c r="B18" s="19" t="s">
         <v>15</v>
       </c>
@@ -3636,9 +3682,12 @@
       <c r="H18" s="57">
         <v>27097874</v>
       </c>
+      <c r="I18" s="22">
+        <v>16</v>
+      </c>
     </row>
     <row r="19" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="78"/>
+      <c r="A19" s="108"/>
       <c r="B19" s="21" t="s">
         <v>20</v>
       </c>
@@ -3660,9 +3709,12 @@
       <c r="H19" s="57">
         <v>35455892.844144106</v>
       </c>
+      <c r="I19" s="22">
+        <v>17</v>
+      </c>
     </row>
     <row r="20" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="78" t="s">
+      <c r="A20" s="108" t="s">
         <v>29</v>
       </c>
       <c r="B20" s="20" t="s">
@@ -3691,9 +3743,12 @@
         <f>H22*H2*1000</f>
         <v>4174465</v>
       </c>
+      <c r="I20" s="22">
+        <v>18</v>
+      </c>
     </row>
     <row r="21" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="78"/>
+      <c r="A21" s="108"/>
       <c r="B21" s="20" t="s">
         <v>28</v>
       </c>
@@ -3720,9 +3775,12 @@
         <f>13233.722944494*1000</f>
         <v>13233722.944494</v>
       </c>
+      <c r="I21" s="22">
+        <v>19</v>
+      </c>
     </row>
     <row r="22" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="78"/>
+      <c r="A22" s="108"/>
       <c r="B22" s="20" t="s">
         <v>28</v>
       </c>
@@ -3749,9 +3807,12 @@
         <f>4174.465/H2</f>
         <v>1.5873878704221283E-3</v>
       </c>
+      <c r="I22" s="22">
+        <v>20</v>
+      </c>
     </row>
     <row r="23" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="78"/>
+      <c r="A23" s="108"/>
       <c r="B23" s="33" t="s">
         <v>27</v>
       </c>
@@ -3763,9 +3824,12 @@
       <c r="F23" s="17"/>
       <c r="G23" s="62"/>
       <c r="H23" s="62"/>
+      <c r="I23" s="22">
+        <v>21</v>
+      </c>
     </row>
     <row r="24" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="78"/>
+      <c r="A24" s="108"/>
       <c r="B24" s="33" t="s">
         <v>27</v>
       </c>
@@ -3777,13 +3841,16 @@
       <c r="F24" s="17"/>
       <c r="G24" s="62"/>
       <c r="H24" s="62"/>
+      <c r="I24" s="22">
+        <v>22</v>
+      </c>
     </row>
     <row r="25" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="78"/>
+      <c r="A25" s="108"/>
       <c r="B25" s="33" t="s">
         <v>27</v>
       </c>
-      <c r="C25" s="92" t="s">
+      <c r="C25" s="85" t="s">
         <v>68</v>
       </c>
       <c r="D25" s="63"/>
@@ -3791,9 +3858,12 @@
       <c r="F25" s="18"/>
       <c r="G25" s="64"/>
       <c r="H25" s="64"/>
+      <c r="I25" s="22">
+        <v>23</v>
+      </c>
     </row>
     <row r="26" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="78"/>
+      <c r="A26" s="108"/>
       <c r="B26" s="33" t="s">
         <v>27</v>
       </c>
@@ -3801,23 +3871,26 @@
         <v>14</v>
       </c>
       <c r="D26" s="42">
-        <v>3.27</v>
+        <v>3.2</v>
       </c>
       <c r="E26" s="42">
-        <v>3.27</v>
+        <v>3.2</v>
       </c>
       <c r="F26" s="42">
-        <v>3.27</v>
+        <v>3.2</v>
       </c>
       <c r="G26" s="42">
-        <v>3.27</v>
+        <v>3.2</v>
       </c>
       <c r="H26" s="42">
-        <v>3.27</v>
+        <v>3.2</v>
+      </c>
+      <c r="I26" s="22">
+        <v>24</v>
       </c>
     </row>
     <row r="27" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="78"/>
+      <c r="A27" s="108"/>
       <c r="B27" s="20" t="s">
         <v>50</v>
       </c>
@@ -3844,9 +3917,12 @@
         <f>896035614/$J$11/H$2</f>
         <v>114.00776411636919</v>
       </c>
+      <c r="I27" s="22">
+        <v>25</v>
+      </c>
     </row>
     <row r="28" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="78"/>
+      <c r="A28" s="108"/>
       <c r="B28" s="20" t="s">
         <v>50</v>
       </c>
@@ -3873,9 +3949,12 @@
         <f>756026*1000/H2</f>
         <v>287.4874989067485</v>
       </c>
+      <c r="I28" s="22">
+        <v>26</v>
+      </c>
     </row>
     <row r="29" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="78"/>
+      <c r="A29" s="108"/>
       <c r="B29" s="20" t="s">
         <v>50</v>
       </c>
@@ -3902,11 +3981,14 @@
         <f>25536070/H2</f>
         <v>9.710381516254273</v>
       </c>
+      <c r="I29" s="22">
+        <v>27</v>
+      </c>
       <c r="J29" s="4"/>
       <c r="K29" s="44"/>
     </row>
     <row r="30" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="78"/>
+      <c r="A30" s="108"/>
       <c r="B30" s="20" t="s">
         <v>18</v>
       </c>
@@ -3918,11 +4000,14 @@
       <c r="F30" s="34"/>
       <c r="G30" s="34"/>
       <c r="H30" s="34"/>
+      <c r="I30" s="22">
+        <v>28</v>
+      </c>
       <c r="J30" s="4"/>
       <c r="K30" s="44"/>
     </row>
     <row r="31" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="78"/>
+      <c r="A31" s="108"/>
       <c r="B31" s="20" t="s">
         <v>18</v>
       </c>
@@ -3934,60 +4019,69 @@
       <c r="F31" s="35"/>
       <c r="G31" s="54"/>
       <c r="H31" s="56"/>
+      <c r="I31" s="22">
+        <v>29</v>
+      </c>
       <c r="J31" s="4"/>
       <c r="K31" s="44"/>
     </row>
-    <row r="32" spans="1:11" s="82" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="78"/>
+    <row r="32" spans="1:11" s="77" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="108"/>
       <c r="B32" s="28" t="s">
         <v>3</v>
       </c>
       <c r="C32" s="36" t="s">
         <v>56</v>
       </c>
-      <c r="D32" s="106">
+      <c r="D32" s="99">
         <v>0.70854616755792676</v>
       </c>
-      <c r="E32" s="106">
+      <c r="E32" s="99">
         <v>0.50971693404635232</v>
       </c>
-      <c r="F32" s="106">
+      <c r="F32" s="99">
         <v>0.46573815073814728</v>
       </c>
-      <c r="G32" s="106">
+      <c r="G32" s="99">
         <v>0.3711947712418322</v>
       </c>
-      <c r="H32" s="106">
+      <c r="H32" s="99">
         <v>0.37987390532251908</v>
       </c>
+      <c r="I32" s="22">
+        <v>30</v>
+      </c>
       <c r="K32" s="45"/>
     </row>
-    <row r="33" spans="1:8" s="82" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="78"/>
+    <row r="33" spans="1:9" s="77" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="108"/>
       <c r="B33" s="28" t="s">
         <v>3</v>
       </c>
       <c r="C33" s="36" t="s">
         <v>64</v>
       </c>
-      <c r="D33" s="106">
+      <c r="D33" s="99">
         <v>7.4234096827093481</v>
       </c>
-      <c r="E33" s="106">
+      <c r="E33" s="99">
         <v>7.5813865811051073</v>
       </c>
-      <c r="F33" s="106">
+      <c r="F33" s="99">
         <v>7.8893812548562892</v>
       </c>
-      <c r="G33" s="106">
+      <c r="G33" s="99">
         <v>7.4143824313725872</v>
       </c>
-      <c r="H33" s="106">
+      <c r="H33" s="99">
         <v>7.5505573491218456</v>
       </c>
-    </row>
-    <row r="34" spans="1:8" s="82" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="78"/>
+      <c r="I33" s="22">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" s="77" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="108"/>
       <c r="B34" s="29" t="s">
         <v>4</v>
       </c>
@@ -3999,9 +4093,12 @@
       <c r="F34" s="30"/>
       <c r="G34" s="66"/>
       <c r="H34" s="66"/>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A35" s="78"/>
+      <c r="I34" s="22">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A35" s="108"/>
       <c r="B35" s="19" t="s">
         <v>70</v>
       </c>
@@ -4023,9 +4120,12 @@
       <c r="H35" s="57">
         <v>9790200</v>
       </c>
-    </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A36" s="78"/>
+      <c r="I35" s="22">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A36" s="108"/>
       <c r="B36" s="19" t="s">
         <v>70</v>
       </c>
@@ -4047,9 +4147,12 @@
       <c r="H36" s="57">
         <v>9324000</v>
       </c>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A37" s="78"/>
+      <c r="I36" s="22">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A37" s="108"/>
       <c r="B37" s="19" t="s">
         <v>70</v>
       </c>
@@ -4057,23 +4160,26 @@
         <v>72</v>
       </c>
       <c r="D37" s="57">
-        <v>1278116</v>
+        <v>419192</v>
       </c>
       <c r="E37" s="57">
-        <v>2057585</v>
+        <v>738033</v>
       </c>
       <c r="F37" s="57">
-        <v>2741522</v>
+        <v>1058118</v>
       </c>
       <c r="G37" s="57">
-        <v>4369700</v>
+        <v>1818644</v>
       </c>
       <c r="H37" s="57">
-        <v>5146257</v>
-      </c>
-    </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A38" s="78"/>
+        <v>2134853</v>
+      </c>
+      <c r="I37" s="22">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A38" s="108"/>
       <c r="B38" s="19" t="s">
         <v>70</v>
       </c>
@@ -4095,9 +4201,12 @@
       <c r="H38" s="57">
         <v>117711</v>
       </c>
-    </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A39" s="78"/>
+      <c r="I38" s="22">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A39" s="108"/>
       <c r="B39" s="19" t="s">
         <v>70</v>
       </c>
@@ -4119,9 +4228,12 @@
       <c r="H39" s="57">
         <v>0</v>
       </c>
-    </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A40" s="78"/>
+      <c r="I39" s="22">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A40" s="108"/>
       <c r="B40" s="19" t="s">
         <v>70</v>
       </c>
@@ -4129,23 +4241,26 @@
         <v>75</v>
       </c>
       <c r="D40" s="57">
-        <v>1068000</v>
+        <v>209076</v>
       </c>
       <c r="E40" s="57">
-        <v>1644170</v>
+        <v>324618</v>
       </c>
       <c r="F40" s="57">
-        <v>2096578</v>
+        <v>413174</v>
       </c>
       <c r="G40" s="57">
-        <v>3156014</v>
+        <v>604958</v>
       </c>
       <c r="H40" s="57">
-        <v>3622126</v>
-      </c>
-    </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A41" s="78"/>
+        <v>610722</v>
+      </c>
+      <c r="I40" s="22">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A41" s="108"/>
       <c r="B41" s="19" t="s">
         <v>70</v>
       </c>
@@ -4166,6 +4281,9 @@
       </c>
       <c r="H41" s="57">
         <v>1406420</v>
+      </c>
+      <c r="I41" s="22">
+        <v>39</v>
       </c>
     </row>
   </sheetData>

</xml_diff>